<commit_message>
Minor changes to SM folder.
</commit_message>
<xml_diff>
--- a/Submissions/Submission 1/Supplementary Materials/master_lighting_data.xlsx
+++ b/Submissions/Submission 1/Supplementary Materials/master_lighting_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Supplementary Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/Submission 1/Supplementary Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6FF39E-D6F2-4D18-8FEB-1C9DAFDE1165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E68869-9425-554C-8EEC-6E2E09A5C75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="642" xr2:uid="{64D75931-346C-4638-8F9E-A211D2C200A3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" tabRatio="642" xr2:uid="{64D75931-346C-4638-8F9E-A211D2C200A3}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Data type</t>
   </si>
@@ -341,6 +341,21 @@
   </si>
   <si>
     <t>This excel workbook is a blank template for use with the R code also supplied in the Supplementary Materials. It will allow for the user to reproduce the results found in this paper for any combination of lamp and weighting function, with data supplied by the user. Data for the weighting functions and lamps used in this study can be found in the sources provided in the data_wf and data_lamp sheets.</t>
+  </si>
+  <si>
+    <t>for the paper</t>
+  </si>
+  <si>
+    <t>by</t>
+  </si>
+  <si>
+    <t>Matthew Kuperus Heun, Zeke Marshall, Emmanuel Aramendia, and Paul E. Brockway</t>
+  </si>
+  <si>
+    <t>submitted to</t>
+  </si>
+  <si>
+    <t>Energies</t>
   </si>
 </sst>
 </file>
@@ -438,15 +453,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -463,10 +478,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -766,137 +777,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFAB5D4-3488-49ED-96A2-D11B459B0BF9}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="116.33203125" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="8"/>
+    <col min="2" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+    <row r="11" spans="1:1" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -904,8 +878,8 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -913,7 +887,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -922,8 +896,10 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -931,8 +907,8 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -940,7 +916,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -949,12 +925,75 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -969,18 +1008,18 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="131.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="131.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1003,8 +1042,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
@@ -1020,8 +1059,8 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B3" t="s">
@@ -1033,11 +1072,11 @@
       <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
@@ -1049,15 +1088,15 @@
       <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>47</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
@@ -1069,7 +1108,7 @@
       <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>52</v>
       </c>
       <c r="G5" t="s">
@@ -1093,13 +1132,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1120,12 +1159,12 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="23.88671875" customWidth="1"/>
+    <col min="1" max="9" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1154,7 +1193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1164,7 +1203,7 @@
       <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>2013</v>
       </c>
       <c r="E2" s="6">
@@ -1177,15 +1216,15 @@
         <f t="shared" ref="G2:G5" si="0">E2*F2</f>
         <v>846</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <f t="shared" ref="H2:H5" si="1">(E2/683)*100</f>
         <v>2.0644216691068813</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1195,7 +1234,7 @@
       <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>2012</v>
       </c>
       <c r="E3" s="6">
@@ -1208,15 +1247,15 @@
         <f t="shared" si="0"/>
         <v>715</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <f t="shared" si="1"/>
         <v>1.6105417276720351</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1226,7 +1265,7 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>2014</v>
       </c>
       <c r="E4" s="6">
@@ -1239,15 +1278,15 @@
         <f t="shared" si="0"/>
         <v>949.5</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <f t="shared" si="1"/>
         <v>9.2679355783308921</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1257,7 +1296,7 @@
       <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>2013</v>
       </c>
       <c r="E5" s="6">
@@ -1270,11 +1309,11 @@
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <f t="shared" si="1"/>
         <v>10.248901903367496</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1297,13 +1336,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Added a reason why we do not republish wf and lamp spd data in the readme sheet.
</commit_message>
<xml_diff>
--- a/Submissions/Submission 1/Supplementary Materials/master_lighting_data.xlsx
+++ b/Submissions/Submission 1/Supplementary Materials/master_lighting_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/LightingPaper2020/Submissions/Submission 1/Supplementary Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\LightingPaper2020\Submissions\Submission 1\Supplementary Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E68869-9425-554C-8EEC-6E2E09A5C75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BC48F0-C20D-4A83-94F0-A956DBAFC016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" tabRatio="642" xr2:uid="{64D75931-346C-4638-8F9E-A211D2C200A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="642" xr2:uid="{64D75931-346C-4638-8F9E-A211D2C200A3}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -340,9 +340,6 @@
     <t>Visible spectrum (380-760nm)</t>
   </si>
   <si>
-    <t>This excel workbook is a blank template for use with the R code also supplied in the Supplementary Materials. It will allow for the user to reproduce the results found in this paper for any combination of lamp and weighting function, with data supplied by the user. Data for the weighting functions and lamps used in this study can be found in the sources provided in the data_wf and data_lamp sheets.</t>
-  </si>
-  <si>
     <t>for the paper</t>
   </si>
   <si>
@@ -356,6 +353,9 @@
   </si>
   <si>
     <t>Energies</t>
+  </si>
+  <si>
+    <t>This excel workbook is a blank template for use with the R code also supplied in the Supplementary Materials. It will allow for the user to reproduce the results found in this paper for any combination of lamp and weighting function, with data supplied by the user. Data for the weighting functions and lamps used in this study can be found in the sources provided in the data_wf and data_lamp sheets. This data was not provided here as is was obtained from open-source datasets produced by other researchers.</t>
   </si>
 </sst>
 </file>
@@ -780,94 +780,94 @@
   <dimension ref="A2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="116.33203125" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="8"/>
+    <col min="2" max="16384" width="8.77734375" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="43.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="15"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>25</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="15"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -887,7 +887,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -896,7 +896,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>26</v>
       </c>
@@ -907,7 +907,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -916,7 +916,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -925,7 +925,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -934,7 +934,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -943,7 +943,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -952,7 +952,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -961,7 +961,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -970,7 +970,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -979,7 +979,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1008,18 +1008,18 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
     <col min="6" max="6" width="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="131.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="131.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>43</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>43</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>43</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -1132,13 +1132,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1159,12 +1159,12 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="23.83203125" customWidth="1"/>
+    <col min="1" max="9" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1336,13 +1336,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>

</xml_diff>